<commit_message>
updates for better bot
</commit_message>
<xml_diff>
--- a/redteaming.xlsx
+++ b/redteaming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BB14738/Desktop/bot copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2CA910-22DF-8549-ADA1-03143725D26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E58B18C-7A83-6141-A1B2-231820054F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Redteaming-All Records-2024-102" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="343">
   <si>
     <t>Question_ID</t>
   </si>
@@ -1058,7 +1058,10 @@
     <t>Explanation5</t>
   </si>
   <si>
-    <t>Explanation6</t>
+    <t>Explanation 6</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -1284,9 +1287,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC6AE013-46D1-384A-A8F7-E7DEB39F8314}" name="Table1" displayName="Table1" ref="A1:R265" totalsRowCount="1" headerRowDxfId="8">
-  <autoFilter ref="A1:R264" xr:uid="{AC6AE013-46D1-384A-A8F7-E7DEB39F8314}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC6AE013-46D1-384A-A8F7-E7DEB39F8314}" name="Table1" displayName="Table1" ref="A1:S265" totalsRowCount="1" headerRowDxfId="8">
+  <autoFilter ref="A1:S264" xr:uid="{AC6AE013-46D1-384A-A8F7-E7DEB39F8314}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{6BA22BE1-4789-B84E-8916-5D7F7FBEFFDE}" name="Question_ID" dataDxfId="7" totalsRowDxfId="3"/>
     <tableColumn id="2" xr3:uid="{23F619C1-81AA-4C4F-8E25-8D95A53F15B1}" name="Question_Type" dataDxfId="6" totalsRowDxfId="2"/>
     <tableColumn id="3" xr3:uid="{7D0B24C7-D948-0C4F-B9EE-F48259997FA6}" name="Question" dataDxfId="5" totalsRowDxfId="1"/>
@@ -1315,7 +1318,8 @@
     <tableColumn id="16" xr3:uid="{074D0ACB-F74F-7C4B-ADB2-790836289617}" name="Bias_Score" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Table1[Bias_Score])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{18186327-BE0A-2F4E-8231-70D59BC6CFB7}" name="Explanation6"/>
+    <tableColumn id="19" xr3:uid="{3938AF67-16EF-3943-B020-46E69A231F82}" name="Explanation 6"/>
+    <tableColumn id="17" xr3:uid="{18186327-BE0A-2F4E-8231-70D59BC6CFB7}" name="Data"/>
     <tableColumn id="18" xr3:uid="{7FC47ECA-5B1F-6C4F-BB7D-D18E85C6224C}" name="Average_Score">
       <calculatedColumnFormula>AVERAGE(F2,H2,J2,L2,N2,P2)</calculatedColumnFormula>
     </tableColumn>
@@ -1525,10 +1529,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R265"/>
+  <dimension ref="A1:S265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P265" sqref="P265"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1547,12 +1551,12 @@
     <col min="13" max="13" width="14.1640625" customWidth="1"/>
     <col min="14" max="14" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="14.1640625" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" customWidth="1"/>
+    <col min="16" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1605,10 +1609,13 @@
         <v>341</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1621,12 +1628,12 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="e">
+      <c r="S2" t="e">
         <f>AVERAGE(F2,H2,J2,L2,N2,P2)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1642,12 +1649,12 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R3" t="e">
-        <f t="shared" ref="R3:R66" si="0">AVERAGE(F3,H3,J3,L3,N3,P3)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S3" t="e">
+        <f t="shared" ref="S3:S66" si="0">AVERAGE(F3,H3,J3,L3,N3,P3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1660,12 +1667,12 @@
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R4" t="e">
+      <c r="S4" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1678,12 +1685,12 @@
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R5" t="e">
+      <c r="S5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1696,12 +1703,12 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R6" t="e">
+      <c r="S6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1714,12 +1721,12 @@
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R7" t="e">
+      <c r="S7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1732,12 +1739,12 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R8" t="e">
+      <c r="S8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1750,12 +1757,12 @@
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R9" t="e">
+      <c r="S9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1768,12 +1775,12 @@
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R10" t="e">
+      <c r="S10" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1786,12 +1793,12 @@
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R11" t="e">
+      <c r="S11" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1804,12 +1811,12 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R12" t="e">
+      <c r="S12" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1825,12 +1832,12 @@
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R13" t="e">
+      <c r="S13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1846,12 +1853,12 @@
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R14" t="e">
+      <c r="S14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1867,12 +1874,12 @@
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R15" t="e">
+      <c r="S15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1888,12 +1895,12 @@
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R16" t="e">
+      <c r="S16" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1909,12 +1916,12 @@
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R17" t="e">
+      <c r="S17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1930,12 +1937,12 @@
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R18" t="e">
+      <c r="S18" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1951,12 +1958,12 @@
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R19" t="e">
+      <c r="S19" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1972,12 +1979,12 @@
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R20" t="e">
+      <c r="S20" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1993,12 +2000,12 @@
       <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R21" t="e">
+      <c r="S21" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2014,12 +2021,12 @@
       <c r="E22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R22" t="e">
+      <c r="S22" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2035,12 +2042,12 @@
       <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R23" t="e">
+      <c r="S23" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2056,12 +2063,12 @@
       <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R24" t="e">
+      <c r="S24" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2077,12 +2084,12 @@
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R25" t="e">
+      <c r="S25" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2098,12 +2105,12 @@
       <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R26" t="e">
+      <c r="S26" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2116,12 +2123,12 @@
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R27" t="e">
+      <c r="S27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2134,12 +2141,12 @@
       <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R28" t="e">
+      <c r="S28" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2152,12 +2159,12 @@
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R29" t="e">
+      <c r="S29" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2170,12 +2177,12 @@
       <c r="E30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R30" t="e">
+      <c r="S30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2188,12 +2195,12 @@
       <c r="E31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R31" t="e">
+      <c r="S31" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2206,12 +2213,12 @@
       <c r="E32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R32" t="e">
+      <c r="S32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2224,12 +2231,12 @@
       <c r="E33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R33" t="e">
+      <c r="S33" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2242,12 +2249,12 @@
       <c r="E34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R34" t="e">
+      <c r="S34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2260,12 +2267,12 @@
       <c r="E35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R35" t="e">
+      <c r="S35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2278,12 +2285,12 @@
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R36" t="e">
+      <c r="S36" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2296,12 +2303,12 @@
       <c r="E37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R37" t="e">
+      <c r="S37" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2314,12 +2321,12 @@
       <c r="E38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R38" t="e">
+      <c r="S38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2332,12 +2339,12 @@
       <c r="E39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R39" t="e">
+      <c r="S39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2350,12 +2357,12 @@
       <c r="E40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R40" t="e">
+      <c r="S40" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2368,12 +2375,12 @@
       <c r="E41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R41" t="e">
+      <c r="S41" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2386,12 +2393,12 @@
       <c r="E42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R42" t="e">
+      <c r="S42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2404,12 +2411,12 @@
       <c r="E43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R43" t="e">
+      <c r="S43" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2422,12 +2429,12 @@
       <c r="E44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R44" t="e">
+      <c r="S44" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2440,12 +2447,12 @@
       <c r="E45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R45" t="e">
+      <c r="S45" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2458,12 +2465,12 @@
       <c r="E46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R46" t="e">
+      <c r="S46" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2476,12 +2483,12 @@
       <c r="E47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R47" t="e">
+      <c r="S47" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2494,12 +2501,12 @@
       <c r="E48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R48" t="e">
+      <c r="S48" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2512,12 +2519,12 @@
       <c r="E49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R49" t="e">
+      <c r="S49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2530,12 +2537,12 @@
       <c r="E50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R50" t="e">
+      <c r="S50" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2548,12 +2555,12 @@
       <c r="E51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R51" t="e">
+      <c r="S51" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2566,12 +2573,12 @@
       <c r="E52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R52" t="e">
+      <c r="S52" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2584,12 +2591,12 @@
       <c r="E53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R53" t="e">
+      <c r="S53" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2602,12 +2609,12 @@
       <c r="E54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R54" t="e">
+      <c r="S54" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2620,12 +2627,12 @@
       <c r="E55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R55" t="e">
+      <c r="S55" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2638,12 +2645,12 @@
       <c r="E56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R56" t="e">
+      <c r="S56" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2656,12 +2663,12 @@
       <c r="E57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R57" t="e">
+      <c r="S57" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2674,12 +2681,12 @@
       <c r="E58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R58" t="e">
+      <c r="S58" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2692,12 +2699,12 @@
       <c r="E59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R59" t="e">
+      <c r="S59" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2710,12 +2717,12 @@
       <c r="E60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R60" t="e">
+      <c r="S60" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2728,12 +2735,12 @@
       <c r="E61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R61" t="e">
+      <c r="S61" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2746,12 +2753,12 @@
       <c r="E62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R62" t="e">
+      <c r="S62" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2764,12 +2771,12 @@
       <c r="E63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R63" t="e">
+      <c r="S63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2782,12 +2789,12 @@
       <c r="E64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R64" t="e">
+      <c r="S64" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2800,12 +2807,12 @@
       <c r="E65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R65" t="e">
+      <c r="S65" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2818,12 +2825,12 @@
       <c r="E66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R66" t="e">
+      <c r="S66" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2836,12 +2843,12 @@
       <c r="E67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R67" t="e">
-        <f t="shared" ref="R67:R130" si="1">AVERAGE(F67,H67,J67,L67,N67,P67)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+      <c r="S67" t="e">
+        <f t="shared" ref="S67:S130" si="1">AVERAGE(F67,H67,J67,L67,N67,P67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2854,12 +2861,12 @@
       <c r="E68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R68" t="e">
+      <c r="S68" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2872,12 +2879,12 @@
       <c r="E69" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R69" t="e">
+      <c r="S69" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2890,12 +2897,12 @@
       <c r="E70" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R70" t="e">
+      <c r="S70" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2908,12 +2915,12 @@
       <c r="E71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R71" t="e">
+      <c r="S71" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2926,12 +2933,12 @@
       <c r="E72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R72" t="e">
+      <c r="S72" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2944,12 +2951,12 @@
       <c r="E73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R73" t="e">
+      <c r="S73" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2962,12 +2969,12 @@
       <c r="E74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R74" t="e">
+      <c r="S74" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2980,12 +2987,12 @@
       <c r="E75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R75" t="e">
+      <c r="S75" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2998,12 +3005,12 @@
       <c r="E76" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R76" t="e">
+      <c r="S76" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3019,12 +3026,12 @@
       <c r="E77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R77" t="e">
+      <c r="S77" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3040,12 +3047,12 @@
       <c r="E78" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R78" t="e">
+      <c r="S78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3061,12 +3068,12 @@
       <c r="E79" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R79" t="e">
+      <c r="S79" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3082,12 +3089,12 @@
       <c r="E80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R80" t="e">
+      <c r="S80" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3103,12 +3110,12 @@
       <c r="E81" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R81" t="e">
+      <c r="S81" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3124,12 +3131,12 @@
       <c r="E82" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R82" t="e">
+      <c r="S82" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3145,12 +3152,12 @@
       <c r="E83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R83" t="e">
+      <c r="S83" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3166,12 +3173,12 @@
       <c r="E84" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R84" t="e">
+      <c r="S84" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3187,12 +3194,12 @@
       <c r="E85" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R85" t="e">
+      <c r="S85" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3208,12 +3215,12 @@
       <c r="E86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R86" t="e">
+      <c r="S86" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3229,12 +3236,12 @@
       <c r="E87" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R87" t="e">
+      <c r="S87" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3250,12 +3257,12 @@
       <c r="E88" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R88" t="e">
+      <c r="S88" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3271,12 +3278,12 @@
       <c r="E89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R89" t="e">
+      <c r="S89" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3292,12 +3299,12 @@
       <c r="E90" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R90" t="e">
+      <c r="S90" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -3313,12 +3320,12 @@
       <c r="E91" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R91" t="e">
+      <c r="S91" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -3334,12 +3341,12 @@
       <c r="E92" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R92" t="e">
+      <c r="S92" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -3355,12 +3362,12 @@
       <c r="E93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R93" t="e">
+      <c r="S93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -3376,12 +3383,12 @@
       <c r="E94" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R94" t="e">
+      <c r="S94" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3397,12 +3404,12 @@
       <c r="E95" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R95" t="e">
+      <c r="S95" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3418,12 +3425,12 @@
       <c r="E96" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R96" t="e">
+      <c r="S96" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -3439,12 +3446,12 @@
       <c r="E97" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R97" t="e">
+      <c r="S97" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -3460,12 +3467,12 @@
       <c r="E98" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R98" t="e">
+      <c r="S98" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -3481,12 +3488,12 @@
       <c r="E99" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R99" t="e">
+      <c r="S99" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3502,12 +3509,12 @@
       <c r="E100" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R100" t="e">
+      <c r="S100" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="101" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3523,12 +3530,12 @@
       <c r="E101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R101" t="e">
+      <c r="S101" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3544,12 +3551,12 @@
       <c r="E102" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R102" t="e">
+      <c r="S102" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3565,12 +3572,12 @@
       <c r="E103" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R103" t="e">
+      <c r="S103" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3586,12 +3593,12 @@
       <c r="E104" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R104" t="e">
+      <c r="S104" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3607,12 +3614,12 @@
       <c r="E105" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R105" t="e">
+      <c r="S105" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -3628,12 +3635,12 @@
       <c r="E106" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R106" t="e">
+      <c r="S106" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -3649,12 +3656,12 @@
       <c r="E107" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R107" t="e">
+      <c r="S107" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -3670,12 +3677,12 @@
       <c r="E108" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R108" t="e">
+      <c r="S108" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -3691,12 +3698,12 @@
       <c r="E109" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R109" t="e">
+      <c r="S109" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -3712,12 +3719,12 @@
       <c r="E110" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R110" t="e">
+      <c r="S110" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -3733,12 +3740,12 @@
       <c r="E111" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R111" t="e">
+      <c r="S111" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3754,12 +3761,12 @@
       <c r="E112" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R112" t="e">
+      <c r="S112" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3775,12 +3782,12 @@
       <c r="E113" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R113" t="e">
+      <c r="S113" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -3796,12 +3803,12 @@
       <c r="E114" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R114" t="e">
+      <c r="S114" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -3817,12 +3824,12 @@
       <c r="E115" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R115" t="e">
+      <c r="S115" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -3838,12 +3845,12 @@
       <c r="E116" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R116" t="e">
+      <c r="S116" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3859,12 +3866,12 @@
       <c r="E117" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R117" t="e">
+      <c r="S117" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -3880,12 +3887,12 @@
       <c r="E118" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R118" t="e">
+      <c r="S118" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3901,12 +3908,12 @@
       <c r="E119" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R119" t="e">
+      <c r="S119" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3922,12 +3929,12 @@
       <c r="E120" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R120" t="e">
+      <c r="S120" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3943,12 +3950,12 @@
       <c r="E121" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R121" t="e">
+      <c r="S121" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3964,12 +3971,12 @@
       <c r="E122" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R122" t="e">
+      <c r="S122" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -3982,12 +3989,12 @@
       <c r="E123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R123" t="e">
+      <c r="S123" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -4000,12 +4007,12 @@
       <c r="E124" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R124" t="e">
+      <c r="S124" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -4018,12 +4025,12 @@
       <c r="E125" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R125" t="e">
+      <c r="S125" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -4036,12 +4043,12 @@
       <c r="E126" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R126" t="e">
+      <c r="S126" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -4054,12 +4061,12 @@
       <c r="E127" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R127" t="e">
+      <c r="S127" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -4072,12 +4079,12 @@
       <c r="E128" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R128" t="e">
+      <c r="S128" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -4090,12 +4097,12 @@
       <c r="E129" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R129" t="e">
+      <c r="S129" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -4108,12 +4115,12 @@
       <c r="E130" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R130" t="e">
+      <c r="S130" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -4126,12 +4133,12 @@
       <c r="E131" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R131" t="e">
-        <f t="shared" ref="R131:R194" si="2">AVERAGE(F131,H131,J131,L131,N131,P131)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+      <c r="S131" t="e">
+        <f t="shared" ref="S131:S194" si="2">AVERAGE(F131,H131,J131,L131,N131,P131)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -4144,12 +4151,12 @@
       <c r="E132" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R132" t="e">
+      <c r="S132" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -4162,12 +4169,12 @@
       <c r="E133" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R133" t="e">
+      <c r="S133" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -4180,12 +4187,12 @@
       <c r="E134" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R134" t="e">
+      <c r="S134" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -4198,12 +4205,12 @@
       <c r="E135" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R135" t="e">
+      <c r="S135" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -4216,12 +4223,12 @@
       <c r="E136" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R136" t="e">
+      <c r="S136" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -4234,12 +4241,12 @@
       <c r="E137" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R137" t="e">
+      <c r="S137" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -4252,12 +4259,12 @@
       <c r="E138" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R138" t="e">
+      <c r="S138" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -4270,12 +4277,12 @@
       <c r="E139" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R139" t="e">
+      <c r="S139" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -4288,12 +4295,12 @@
       <c r="E140" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R140" t="e">
+      <c r="S140" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -4306,12 +4313,12 @@
       <c r="E141" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R141" t="e">
+      <c r="S141" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -4324,12 +4331,12 @@
       <c r="E142" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R142" t="e">
+      <c r="S142" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -4342,12 +4349,12 @@
       <c r="E143" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R143" t="e">
+      <c r="S143" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -4360,12 +4367,12 @@
       <c r="E144" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R144" t="e">
+      <c r="S144" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -4378,12 +4385,12 @@
       <c r="E145" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R145" t="e">
+      <c r="S145" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -4396,12 +4403,12 @@
       <c r="E146" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R146" t="e">
+      <c r="S146" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -4414,12 +4421,12 @@
       <c r="E147" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R147" t="e">
+      <c r="S147" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -4432,12 +4439,12 @@
       <c r="E148" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R148" t="e">
+      <c r="S148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -4450,12 +4457,12 @@
       <c r="E149" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R149" t="e">
+      <c r="S149" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -4468,12 +4475,12 @@
       <c r="E150" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R150" t="e">
+      <c r="S150" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="151" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -4486,12 +4493,12 @@
       <c r="E151" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R151" t="e">
+      <c r="S151" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -4504,12 +4511,12 @@
       <c r="E152" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R152" t="e">
+      <c r="S152" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="153" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -4522,12 +4529,12 @@
       <c r="E153" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R153" t="e">
+      <c r="S153" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="154" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -4540,12 +4547,12 @@
       <c r="E154" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R154" t="e">
+      <c r="S154" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="155" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -4558,12 +4565,12 @@
       <c r="E155" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R155" t="e">
+      <c r="S155" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -4576,12 +4583,12 @@
       <c r="E156" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R156" t="e">
+      <c r="S156" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -4594,12 +4601,12 @@
       <c r="E157" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R157" t="e">
+      <c r="S157" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="158" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -4612,12 +4619,12 @@
       <c r="E158" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R158" t="e">
+      <c r="S158" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -4630,12 +4637,12 @@
       <c r="E159" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R159" t="e">
+      <c r="S159" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -4648,12 +4655,12 @@
       <c r="E160" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R160" t="e">
+      <c r="S160" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="161" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -4666,12 +4673,12 @@
       <c r="E161" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R161" t="e">
+      <c r="S161" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="162" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -4684,12 +4691,12 @@
       <c r="E162" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R162" t="e">
+      <c r="S162" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="163" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -4702,12 +4709,12 @@
       <c r="E163" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R163" t="e">
+      <c r="S163" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="164" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -4720,12 +4727,12 @@
       <c r="E164" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R164" t="e">
+      <c r="S164" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="165" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4738,12 +4745,12 @@
       <c r="E165" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R165" t="e">
+      <c r="S165" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="166" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -4756,12 +4763,12 @@
       <c r="E166" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R166" t="e">
+      <c r="S166" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="167" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -4774,12 +4781,12 @@
       <c r="E167" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R167" t="e">
+      <c r="S167" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="168" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -4792,12 +4799,12 @@
       <c r="E168" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R168" t="e">
+      <c r="S168" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="169" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -4810,12 +4817,12 @@
       <c r="E169" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R169" t="e">
+      <c r="S169" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="170" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -4828,12 +4835,12 @@
       <c r="E170" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R170" t="e">
+      <c r="S170" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="171" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -4846,12 +4853,12 @@
       <c r="E171" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R171" t="e">
+      <c r="S171" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="172" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -4864,12 +4871,12 @@
       <c r="E172" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R172" t="e">
+      <c r="S172" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="173" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -4882,12 +4889,12 @@
       <c r="E173" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R173" t="e">
+      <c r="S173" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="174" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4900,12 +4907,12 @@
       <c r="E174" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R174" t="e">
+      <c r="S174" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="175" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -4918,12 +4925,12 @@
       <c r="E175" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R175" t="e">
+      <c r="S175" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="176" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4936,12 +4943,12 @@
       <c r="E176" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R176" t="e">
+      <c r="S176" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="177" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -4954,12 +4961,12 @@
       <c r="E177" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R177" t="e">
+      <c r="S177" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="178" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -4972,12 +4979,12 @@
       <c r="E178" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R178" t="e">
+      <c r="S178" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="179" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -4990,12 +4997,12 @@
       <c r="E179" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R179" t="e">
+      <c r="S179" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="180" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -5008,12 +5015,12 @@
       <c r="E180" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R180" t="e">
+      <c r="S180" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="181" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -5026,12 +5033,12 @@
       <c r="E181" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R181" t="e">
+      <c r="S181" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="182" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -5044,12 +5051,12 @@
       <c r="E182" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R182" t="e">
+      <c r="S182" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="183" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -5062,12 +5069,12 @@
       <c r="E183" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R183" t="e">
+      <c r="S183" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="184" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -5080,12 +5087,12 @@
       <c r="E184" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R184" t="e">
+      <c r="S184" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="185" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -5098,12 +5105,12 @@
       <c r="E185" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R185" t="e">
+      <c r="S185" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="186" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -5116,12 +5123,12 @@
       <c r="E186" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R186" t="e">
+      <c r="S186" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="187" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -5134,12 +5141,12 @@
       <c r="E187" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R187" t="e">
+      <c r="S187" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="188" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -5152,12 +5159,12 @@
       <c r="E188" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R188" t="e">
+      <c r="S188" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="189" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -5170,12 +5177,12 @@
       <c r="E189" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R189" t="e">
+      <c r="S189" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="190" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -5188,12 +5195,12 @@
       <c r="E190" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R190" t="e">
+      <c r="S190" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="191" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -5206,12 +5213,12 @@
       <c r="E191" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R191" t="e">
+      <c r="S191" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="192" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -5224,12 +5231,12 @@
       <c r="E192" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R192" t="e">
+      <c r="S192" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -5242,12 +5249,12 @@
       <c r="E193" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R193" t="e">
+      <c r="S193" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="194" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -5260,12 +5267,12 @@
       <c r="E194" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R194" t="e">
+      <c r="S194" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -5278,12 +5285,12 @@
       <c r="E195" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R195" t="e">
-        <f t="shared" ref="R195:R258" si="3">AVERAGE(F195,H195,J195,L195,N195,P195)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="196" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+      <c r="S195" t="e">
+        <f t="shared" ref="S195:S258" si="3">AVERAGE(F195,H195,J195,L195,N195,P195)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="196" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -5296,12 +5303,12 @@
       <c r="E196" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R196" t="e">
+      <c r="S196" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="197" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -5314,12 +5321,12 @@
       <c r="E197" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R197" t="e">
+      <c r="S197" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="198" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -5332,12 +5339,12 @@
       <c r="E198" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R198" t="e">
+      <c r="S198" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -5350,12 +5357,12 @@
       <c r="E199" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R199" t="e">
+      <c r="S199" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="200" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -5368,12 +5375,12 @@
       <c r="E200" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R200" t="e">
+      <c r="S200" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -5386,12 +5393,12 @@
       <c r="E201" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R201" t="e">
+      <c r="S201" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="202" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -5404,12 +5411,12 @@
       <c r="E202" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R202" t="e">
+      <c r="S202" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="203" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -5422,12 +5429,12 @@
       <c r="E203" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R203" t="e">
+      <c r="S203" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -5440,12 +5447,12 @@
       <c r="E204" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R204" t="e">
+      <c r="S204" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -5458,12 +5465,12 @@
       <c r="E205" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R205" t="e">
+      <c r="S205" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="206" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -5476,12 +5483,12 @@
       <c r="E206" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R206" t="e">
+      <c r="S206" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="207" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -5494,12 +5501,12 @@
       <c r="E207" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R207" t="e">
+      <c r="S207" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="208" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -5512,12 +5519,12 @@
       <c r="E208" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R208" t="e">
+      <c r="S208" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="209" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -5530,12 +5537,12 @@
       <c r="E209" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R209" t="e">
+      <c r="S209" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="210" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -5548,12 +5555,12 @@
       <c r="E210" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R210" t="e">
+      <c r="S210" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -5566,12 +5573,12 @@
       <c r="E211" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R211" t="e">
+      <c r="S211" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -5584,12 +5591,12 @@
       <c r="E212" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R212" t="e">
+      <c r="S212" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="213" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -5602,12 +5609,12 @@
       <c r="E213" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R213" t="e">
+      <c r="S213" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -5620,12 +5627,12 @@
       <c r="E214" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R214" t="e">
+      <c r="S214" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -5638,12 +5645,12 @@
       <c r="E215" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R215" t="e">
+      <c r="S215" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -5656,12 +5663,12 @@
       <c r="E216" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R216" t="e">
+      <c r="S216" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="217" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -5674,12 +5681,12 @@
       <c r="E217" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R217" t="e">
+      <c r="S217" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -5692,12 +5699,12 @@
       <c r="E218" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R218" t="e">
+      <c r="S218" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -5710,12 +5717,12 @@
       <c r="E219" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R219" t="e">
+      <c r="S219" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -5728,12 +5735,12 @@
       <c r="E220" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R220" t="e">
+      <c r="S220" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -5746,12 +5753,12 @@
       <c r="E221" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R221" t="e">
+      <c r="S221" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -5764,12 +5771,12 @@
       <c r="E222" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R222" t="e">
+      <c r="S222" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -5782,12 +5789,12 @@
       <c r="E223" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R223" t="e">
+      <c r="S223" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="224" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -5800,12 +5807,12 @@
       <c r="E224" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R224" t="e">
+      <c r="S224" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="225" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -5818,12 +5825,12 @@
       <c r="E225" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R225" t="e">
+      <c r="S225" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="226" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -5836,12 +5843,12 @@
       <c r="E226" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R226" t="e">
+      <c r="S226" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="227" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -5854,12 +5861,12 @@
       <c r="E227" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R227" t="e">
+      <c r="S227" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="228" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -5872,12 +5879,12 @@
       <c r="E228" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R228" t="e">
+      <c r="S228" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="229" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -5890,12 +5897,12 @@
       <c r="E229" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R229" t="e">
+      <c r="S229" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="230" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -5908,12 +5915,12 @@
       <c r="E230" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R230" t="e">
+      <c r="S230" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="231" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -5926,12 +5933,12 @@
       <c r="E231" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R231" t="e">
+      <c r="S231" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="232" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -5944,12 +5951,12 @@
       <c r="E232" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R232" t="e">
+      <c r="S232" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="233" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -5962,12 +5969,12 @@
       <c r="E233" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R233" t="e">
+      <c r="S233" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="234" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -5980,12 +5987,12 @@
       <c r="E234" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R234" t="e">
+      <c r="S234" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="235" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -5998,12 +6005,12 @@
       <c r="E235" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R235" t="e">
+      <c r="S235" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="236" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -6016,12 +6023,12 @@
       <c r="E236" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R236" t="e">
+      <c r="S236" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="237" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -6034,12 +6041,12 @@
       <c r="E237" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R237" t="e">
+      <c r="S237" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="238" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -6052,12 +6059,12 @@
       <c r="E238" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R238" t="e">
+      <c r="S238" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="239" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -6070,12 +6077,12 @@
       <c r="E239" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R239" t="e">
+      <c r="S239" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="240" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -6088,12 +6095,12 @@
       <c r="E240" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R240" t="e">
+      <c r="S240" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="241" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -6106,12 +6113,12 @@
       <c r="E241" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R241" t="e">
+      <c r="S241" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="242" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -6124,12 +6131,12 @@
       <c r="E242" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R242" t="e">
+      <c r="S242" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="243" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -6142,12 +6149,12 @@
       <c r="E243" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R243" t="e">
+      <c r="S243" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="244" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -6160,12 +6167,12 @@
       <c r="E244" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R244" t="e">
+      <c r="S244" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="245" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -6178,12 +6185,12 @@
       <c r="E245" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R245" t="e">
+      <c r="S245" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="246" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -6196,12 +6203,12 @@
       <c r="E246" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R246" t="e">
+      <c r="S246" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="247" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -6214,12 +6221,12 @@
       <c r="E247" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R247" t="e">
+      <c r="S247" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="248" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -6232,12 +6239,12 @@
       <c r="E248" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R248" t="e">
+      <c r="S248" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="249" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -6250,12 +6257,12 @@
       <c r="E249" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R249" t="e">
+      <c r="S249" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="250" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -6268,12 +6275,12 @@
       <c r="E250" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R250" t="e">
+      <c r="S250" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="251" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -6286,12 +6293,12 @@
       <c r="E251" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R251" t="e">
+      <c r="S251" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="252" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -6304,12 +6311,12 @@
       <c r="E252" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R252" t="e">
+      <c r="S252" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="253" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -6322,12 +6329,12 @@
       <c r="E253" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R253" t="e">
+      <c r="S253" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="254" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -6340,12 +6347,12 @@
       <c r="E254" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R254" t="e">
+      <c r="S254" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="255" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -6358,12 +6365,12 @@
       <c r="E255" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R255" t="e">
+      <c r="S255" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="256" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -6376,12 +6383,12 @@
       <c r="E256" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R256" t="e">
+      <c r="S256" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="257" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -6394,12 +6401,12 @@
       <c r="E257" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R257" t="e">
+      <c r="S257" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="258" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -6412,12 +6419,12 @@
       <c r="E258" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R258" t="e">
+      <c r="S258" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="259" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -6430,12 +6437,12 @@
       <c r="E259" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R259" t="e">
-        <f t="shared" ref="R259:R264" si="4">AVERAGE(F259,H259,J259,L259,N259,P259)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="260" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+      <c r="S259" t="e">
+        <f t="shared" ref="S259:S264" si="4">AVERAGE(F259,H259,J259,L259,N259,P259)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="260" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -6448,12 +6455,12 @@
       <c r="E260" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R260" t="e">
+      <c r="S260" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="261" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -6466,12 +6473,12 @@
       <c r="E261" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R261" t="e">
+      <c r="S261" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="262" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -6484,12 +6491,12 @@
       <c r="E262" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R262" t="e">
+      <c r="S262" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="263" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -6502,12 +6509,12 @@
       <c r="E263" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R263" t="e">
+      <c r="S263" t="e">
         <f>AVERAGE(F263,H263,J263,L263,N263,P263)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="264" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:19" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -6520,12 +6527,12 @@
       <c r="E264" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R264" t="e">
+      <c r="S264" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="265" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>

</xml_diff>